<commit_message>
cronograma de entregas sinalizado
</commit_message>
<xml_diff>
--- a/Cronograma de Entregas.xlsx
+++ b/Cronograma de Entregas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\O meu disco\Documents\Universidade\LESIPL3ano\1Semestre\ProjetoAplicado\PA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\Projects\ProjetoAplicado\PA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AFC89A-EC58-4DA9-80E8-B9FF05AB92D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C195526-0470-4E0B-8F65-8960906D98E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,14 +576,14 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,7 +904,7 @@
   </sheetPr>
   <dimension ref="A1:Q924"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="O88" sqref="O88"/>
     </sheetView>
   </sheetViews>
@@ -965,38 +965,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="36"/>
+      <c r="F3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="36"/>
+      <c r="J3" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="36"/>
+      <c r="L3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="37" t="s">
+      <c r="M3" s="36"/>
+      <c r="N3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="37" t="s">
+      <c r="O3" s="36"/>
+      <c r="P3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="36"/>
     </row>
     <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="9">
@@ -1035,7 +1035,7 @@
     </row>
     <row r="5" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
-      <c r="B5" s="36"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="6" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="37" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -1113,7 +1113,7 @@
     </row>
     <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
-      <c r="B7" s="36"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="9">
         <v>2</v>
       </c>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
-      <c r="B8" s="36"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="9">
         <v>3</v>
       </c>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
-      <c r="B9" s="36"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="9">
         <v>4</v>
       </c>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="9">
@@ -1259,7 +1259,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
-      <c r="B11" s="36"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="9">
         <v>6</v>
       </c>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
-      <c r="B12" s="36"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="9">
         <v>7</v>
       </c>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
-      <c r="B13" s="36"/>
+      <c r="B13" s="38"/>
       <c r="C13" s="9">
         <v>8</v>
       </c>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9">
@@ -1401,7 +1401,7 @@
     </row>
     <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
-      <c r="B15" s="36"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="9">
         <v>10</v>
       </c>
@@ -1438,7 +1438,7 @@
     </row>
     <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
-      <c r="B16" s="36"/>
+      <c r="B16" s="38"/>
       <c r="C16" s="9">
         <v>11</v>
       </c>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="17" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
-      <c r="B17" s="36"/>
+      <c r="B17" s="38"/>
       <c r="C17" s="9">
         <v>12</v>
       </c>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="18" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
-      <c r="B18" s="36"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="9">
         <v>13</v>
       </c>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="19" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="9">
@@ -1580,7 +1580,7 @@
     </row>
     <row r="20" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
-      <c r="B20" s="36"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="9">
         <v>15</v>
       </c>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="21" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
-      <c r="B21" s="36"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="9">
         <v>16</v>
       </c>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="22" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
-      <c r="B22" s="36"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="9">
         <v>17</v>
       </c>
@@ -6474,6 +6474,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6481,11 +6486,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
review entrega 2 update
</commit_message>
<xml_diff>
--- a/Cronograma de Entregas.xlsx
+++ b/Cronograma de Entregas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\Projects\ProjetoAplicado\PA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\Projects\ProjetoAplicado\SmartBar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49498A2-C237-4ADE-B82B-E3656413DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D04E87-67D4-4AB1-AB89-46AC529B266D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="473" windowWidth="15390" windowHeight="9442" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="3" r:id="rId1"/>
@@ -512,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -576,14 +576,15 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:Q923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -965,38 +966,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="35" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="35" t="s">
+      <c r="I3" s="38"/>
+      <c r="J3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="36"/>
-      <c r="L3" s="35" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="35" t="s">
+      <c r="M3" s="38"/>
+      <c r="N3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="35" t="s">
+      <c r="O3" s="38"/>
+      <c r="P3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="36"/>
+      <c r="Q3" s="38"/>
     </row>
     <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="9">
@@ -1035,7 +1036,7 @@
     </row>
     <row r="5" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="4"/>
-      <c r="B5" s="38"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
@@ -1074,7 +1075,7 @@
     </row>
     <row r="6" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="4"/>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -1113,7 +1114,7 @@
     </row>
     <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
-      <c r="B7" s="38"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="9">
         <v>2</v>
       </c>
@@ -1152,7 +1153,7 @@
     </row>
     <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
-      <c r="B8" s="38"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="9">
         <v>3</v>
       </c>
@@ -1188,7 +1189,7 @@
     </row>
     <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
-      <c r="B9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="9">
         <v>4</v>
       </c>
@@ -1223,7 +1224,7 @@
     </row>
     <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="4"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="9">
@@ -1259,7 +1260,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
-      <c r="B11" s="38"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="9">
         <v>6</v>
       </c>
@@ -1294,7 +1295,7 @@
     </row>
     <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
-      <c r="B12" s="38"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="9">
         <v>7</v>
       </c>
@@ -1330,7 +1331,7 @@
     </row>
     <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="4"/>
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="9">
         <v>8</v>
       </c>
@@ -1365,7 +1366,7 @@
     </row>
     <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="4"/>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="35" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9">
@@ -1401,7 +1402,7 @@
     </row>
     <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="4"/>
-      <c r="B15" s="38"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="9">
         <v>10</v>
       </c>
@@ -1438,7 +1439,7 @@
     </row>
     <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="4"/>
-      <c r="B16" s="38"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="9">
         <v>11</v>
       </c>
@@ -1471,7 +1472,7 @@
     </row>
     <row r="17" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="4"/>
-      <c r="B17" s="38"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="9">
         <v>12</v>
       </c>
@@ -1506,7 +1507,7 @@
     </row>
     <row r="18" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="4"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="9">
         <v>13</v>
       </c>
@@ -1541,7 +1542,7 @@
     </row>
     <row r="19" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="4"/>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="9">
@@ -1580,7 +1581,7 @@
     </row>
     <row r="20" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="4"/>
-      <c r="B20" s="38"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="9">
         <v>15</v>
       </c>
@@ -1617,7 +1618,7 @@
     </row>
     <row r="21" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="4"/>
-      <c r="B21" s="38"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="9">
         <v>16</v>
       </c>
@@ -1662,7 +1663,7 @@
     </row>
     <row r="22" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="4"/>
-      <c r="B22" s="38"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="9">
         <v>17</v>
       </c>
@@ -2031,9 +2032,14 @@
       <c r="A58" s="23"/>
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
-      <c r="G58" s="31" t="s">
+      <c r="G58" s="39" t="s">
         <v>81</v>
       </c>
+      <c r="H58" s="33"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A59" s="23"/>
@@ -6498,11 +6504,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6510,6 +6511,11 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
relatorio entrega 3 final
</commit_message>
<xml_diff>
--- a/Cronograma de Entregas.xlsx
+++ b/Cronograma de Entregas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\Projects\ProjetoAplicado\SmartBar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC69AF8B-B9FD-4A72-B5FA-AD094EEE3E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFA2A2B-7A12-4C10-8B39-8706F3871834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25770" yWindow="930" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,14 +577,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,7 +906,7 @@
   <dimension ref="A1:Q923"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+      <selection activeCell="G66" sqref="G66:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -966,38 +966,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36" t="s">
+      <c r="K3" s="39"/>
+      <c r="L3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="36" t="s">
+      <c r="M3" s="39"/>
+      <c r="N3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="36" t="s">
+      <c r="O3" s="39"/>
+      <c r="P3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="37"/>
+      <c r="Q3" s="39"/>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="9">
@@ -1036,7 +1036,7 @@
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="39"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -1114,7 +1114,7 @@
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="39"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="9">
         <v>2</v>
       </c>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="39"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="9">
         <v>3</v>
       </c>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="39"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="9">
         <v>4</v>
       </c>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="9">
@@ -1260,7 +1260,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="39"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="9">
         <v>6</v>
       </c>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="39"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="9">
         <v>7</v>
       </c>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="39"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="9">
         <v>8</v>
       </c>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="36" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9">
@@ -1402,7 +1402,7 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="39"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="9">
         <v>10</v>
       </c>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="39"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="9">
         <v>11</v>
       </c>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="39"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="9">
         <v>12</v>
       </c>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="39"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="9">
         <v>13</v>
       </c>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="9">
@@ -1581,7 +1581,7 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="39"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="9">
         <v>15</v>
       </c>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="39"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="9">
         <v>16</v>
       </c>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="39"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="9">
         <v>17</v>
       </c>
@@ -2136,9 +2136,13 @@
       <c r="A66" s="23"/>
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
-      <c r="G66" s="31" t="s">
+      <c r="G66" s="35" t="s">
         <v>82</v>
       </c>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
@@ -2168,33 +2172,49 @@
       <c r="A69" s="23"/>
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
-      <c r="G69" s="30" t="s">
+      <c r="G69" s="32" t="s">
         <v>66</v>
       </c>
+      <c r="H69" s="33"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33"/>
+      <c r="K69" s="33"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
-      <c r="G70" s="30" t="s">
+      <c r="G70" s="32" t="s">
         <v>67</v>
       </c>
+      <c r="H70" s="33"/>
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+      <c r="K70" s="33"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
-      <c r="G71" s="30" t="s">
+      <c r="G71" s="32" t="s">
         <v>55</v>
       </c>
+      <c r="H71" s="33"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+      <c r="K71" s="33"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="23"/>
       <c r="B72" s="24"/>
       <c r="C72" s="24"/>
-      <c r="H72" s="30" t="s">
+      <c r="G72" s="33"/>
+      <c r="H72" s="32" t="s">
         <v>61</v>
       </c>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
+      <c r="K72" s="33"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
@@ -6519,11 +6539,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6531,6 +6546,11 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
update controller entrega backend
</commit_message>
<xml_diff>
--- a/Cronograma de Entregas.xlsx
+++ b/Cronograma de Entregas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pessoal\Projects\ProjetoAplicado\SmartBar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFA2A2B-7A12-4C10-8B39-8706F3871834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A947F0E0-7C7B-4B84-B9A2-215A5A51938D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25770" yWindow="930" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5730" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="3" r:id="rId1"/>
@@ -577,14 +577,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:Q923"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66:K66"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -966,38 +966,38 @@
       <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="38" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="38" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="38" t="s">
+      <c r="O3" s="37"/>
+      <c r="P3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="39"/>
+      <c r="Q3" s="37"/>
     </row>
     <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="9">
@@ -1036,7 +1036,7 @@
     </row>
     <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="9">
@@ -1114,7 +1114,7 @@
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="37"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="9">
         <v>2</v>
       </c>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="37"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="9">
         <v>3</v>
       </c>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="37"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="9">
         <v>4</v>
       </c>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="38" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="9">
@@ -1260,7 +1260,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="37"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="9">
         <v>6</v>
       </c>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="37"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="9">
         <v>7</v>
       </c>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="37"/>
+      <c r="B13" s="39"/>
       <c r="C13" s="9">
         <v>8</v>
       </c>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9">
@@ -1402,7 +1402,7 @@
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="37"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="9">
         <v>10</v>
       </c>
@@ -1439,7 +1439,7 @@
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="37"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="9">
         <v>11</v>
       </c>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="37"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="9">
         <v>12</v>
       </c>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="37"/>
+      <c r="B18" s="39"/>
       <c r="C18" s="9">
         <v>13</v>
       </c>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="9">
@@ -1581,7 +1581,7 @@
     </row>
     <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="37"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="9">
         <v>15</v>
       </c>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="37"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="9">
         <v>16</v>
       </c>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="37"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="9">
         <v>17</v>
       </c>
@@ -2226,33 +2226,49 @@
       <c r="A74" s="23"/>
       <c r="B74" s="24"/>
       <c r="C74" s="24"/>
-      <c r="G74" s="31" t="s">
+      <c r="G74" s="35" t="s">
         <v>83</v>
       </c>
+      <c r="H74" s="33"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="33"/>
+      <c r="K74" s="33"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="23"/>
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
-      <c r="G75" s="30" t="s">
+      <c r="G75" s="32" t="s">
         <v>68</v>
       </c>
+      <c r="H75" s="33"/>
+      <c r="I75" s="33"/>
+      <c r="J75" s="33"/>
+      <c r="K75" s="33"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="23"/>
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
-      <c r="G76" s="30" t="s">
+      <c r="G76" s="32" t="s">
         <v>69</v>
       </c>
+      <c r="H76" s="33"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="23"/>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
-      <c r="H77" s="30" t="s">
+      <c r="G77" s="33"/>
+      <c r="H77" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="I77" s="33"/>
+      <c r="J77" s="33"/>
+      <c r="K77" s="33"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="23"/>
@@ -6539,6 +6555,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B18"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="F3:G3"/>
@@ -6546,11 +6567,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>